<commit_message>
Fungerer med spilleliste til vlc
</commit_message>
<xml_diff>
--- a/output/Startliste_FSMData_02-09-2026_KUNSTLØP Oppvisning Bergen.xlsx
+++ b/output/Startliste_FSMData_02-09-2026_KUNSTLØP Oppvisning Bergen.xlsx
@@ -449,7 +449,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Oppvisningsstevne iskanten 9 februar 2026</t>
+          <t>Oppvisningsstevne Iskanten 9 februar 2026</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>17:29:20</t>
+          <t>17:04:00</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>17:00:00</t>
+          <t>17:04:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -521,17 +521,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17:03:40</t>
+          <t>17:07:44</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Frida Qianlu He</t>
+          <t>Elena Sophia Sandnes-Strømmen</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Fana Idrettslag</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17:03:40</t>
+          <t>17:07:44</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -551,17 +551,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>17:07:20</t>
+          <t>17:11:28</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Eleanora Egle</t>
+          <t>Eira Olava Bortne Ludvigsen</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Bergen Kunstløpklubb</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>17:07:20</t>
+          <t>17:11:28</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -581,17 +581,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>17:11:00</t>
+          <t>17:15:12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Valentina Pinker-Spilde</t>
+          <t>Sara Barbro Kyte</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Fana Idrettslag</t>
+          <t>Bergen Kunstløpklubb</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17:11:00</t>
+          <t>17:15:12</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -611,12 +611,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>17:14:40</t>
+          <t>17:18:56</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Sara Barbro Kyte</t>
+          <t>Mie Mariell Sævereid</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17:14:40</t>
+          <t>17:18:56</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -641,12 +641,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>17:18:20</t>
+          <t>17:22:40</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Leah Kalvik</t>
+          <t>Amanda Ansnes Lima</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17:18:20</t>
+          <t>17:22:40</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -671,12 +671,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>17:22:00</t>
+          <t>17:26:24</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Elena Sophia Sandnes-Strømmen</t>
+          <t>Emilie Morseth</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17:22:00</t>
+          <t>17:26:24</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -701,17 +701,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>17:25:40</t>
+          <t>17:30:08</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Patricija Levickaite</t>
+          <t>Leah Kalvik</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Bergen Kunstløpklubb</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17:25:40</t>
+          <t>17:30:08</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -731,17 +731,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>17:29:20</t>
+          <t>17:33:52</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Anne Kristoffersen</t>
+          <t>Aurelia Landschulze</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Fana Idrettslag</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       <c r="A13" s="2" t="inlineStr"/>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>ca. 17:29:20</t>
+          <t>ca. 17:33:52</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>17:58:40</t>
+          <t>17:37:52</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>17:29:20</t>
+          <t>17:37:52</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -785,17 +785,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>17:33:00</t>
+          <t>17:41:36</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Frida Pasko Hansen</t>
+          <t>Sarolt Szofia Papdi</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Bergen Kunstløpklubb</t>
         </is>
       </c>
     </row>
@@ -805,7 +805,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17:33:00</t>
+          <t>17:41:36</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -815,12 +815,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>17:36:40</t>
+          <t>17:45:20</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Hanna Wangsuk Tveita</t>
+          <t>Camilla Tveit</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -835,7 +835,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>17:36:40</t>
+          <t>17:45:20</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -845,17 +845,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>17:40:20</t>
+          <t>17:49:04</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Mie Mariell Sævereid</t>
+          <t>Hanna Wangsuk Tveita</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Bergen Kunstløpklubb</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -865,7 +865,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>17:40:20</t>
+          <t>17:49:04</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -875,12 +875,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>17:44:00</t>
+          <t>17:52:48</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Frida Lovisa Østerberg</t>
+          <t>Patricija Levickaite</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -895,7 +895,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>17:44:00</t>
+          <t>17:52:48</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -905,17 +905,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>17:47:40</t>
+          <t>17:56:32</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Amanda Ansnes Lima</t>
+          <t>Hennie Markestad</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Bergen Kunstløpklubb</t>
         </is>
       </c>
     </row>
@@ -925,7 +925,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17:47:40</t>
+          <t>17:56:32</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -935,7 +935,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>17:51:20</t>
+          <t>18:00:16</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -955,7 +955,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>17:51:20</t>
+          <t>18:00:16</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -965,17 +965,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>17:55:00</t>
+          <t>18:04:00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Eira Olava Bortne Ludvigsen</t>
+          <t>Aylin Morseth</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Bergen Kunstløpklubb</t>
+          <t>Fana Idrettslag</t>
         </is>
       </c>
     </row>
@@ -985,7 +985,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>17:55:00</t>
+          <t>18:04:00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -995,12 +995,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>17:58:40</t>
+          <t>18:07:44</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Camilla Tveit</t>
+          <t>Anne Kristoffersen</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1013,7 +1013,7 @@
       <c r="A22" s="2" t="inlineStr"/>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>ca. 17:58:40</t>
+          <t>ca. 18:07:44</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>18:28:00</t>
+          <t>18:11:44</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>17:58:40</t>
+          <t>18:11:44</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1049,17 +1049,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>18:02:20</t>
+          <t>18:15:28</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Hennie Markestad</t>
+          <t>Angela Chen</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Bergen Kunstløpklubb</t>
+          <t>Fana Idrettslag</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>18:02:20</t>
+          <t>18:15:28</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1079,17 +1079,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>18:06:00</t>
+          <t>18:19:12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Aksel Eriksen</t>
+          <t>Frida Lovisa Østerberg</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Bergen Kunstløpklubb</t>
         </is>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>18:06:00</t>
+          <t>18:19:12</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1109,17 +1109,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>18:09:40</t>
+          <t>18:22:56</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Aylin Morseth</t>
+          <t>Eleanora Egle</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Fana Idrettslag</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>18:09:40</t>
+          <t>18:22:56</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1139,17 +1139,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>18:13:20</t>
+          <t>18:26:40</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Aurelia Landschulze</t>
+          <t>Frida Qianlu He</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Fana Idrettslag</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>18:13:20</t>
+          <t>18:26:40</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1169,17 +1169,17 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>18:17:00</t>
+          <t>18:30:24</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Emilie Morseth</t>
+          <t>Frida Pasko Hansen</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Fana Idrettslag</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>18:17:00</t>
+          <t>18:30:24</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1199,12 +1199,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>18:20:40</t>
+          <t>18:34:08</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Mille Isabell Steen Rein</t>
+          <t>Aksel Eriksen</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>18:20:40</t>
+          <t>18:34:08</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1229,17 +1229,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>18:24:20</t>
+          <t>18:37:52</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Sarolt Szofia Papdi</t>
+          <t>Valentina Pinker-Spilde</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Bergen Kunstløpklubb</t>
+          <t>Fana Idrettslag</t>
         </is>
       </c>
     </row>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>18:24:20</t>
+          <t>18:37:52</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1259,24 +1259,24 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>18:28:00</t>
+          <t>18:41:36</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Angela Chen</t>
+          <t>Mille Isabell Steen Rein</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Fana Idrettslag</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Generert 31.01.2026 22:32</t>
+          <t>Generert 31.01.2026 23:53</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
la til vannmerke med datamaskin navn på startliste
</commit_message>
<xml_diff>
--- a/output/Startliste_FSMData_02-09-2026_KUNSTLØP Oppvisning Bergen.xlsx
+++ b/output/Startliste_FSMData_02-09-2026_KUNSTLØP Oppvisning Bergen.xlsx
@@ -449,7 +449,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Oppvisningsstevne Iskanten 9 februar 2026</t>
+          <t>Oppvisningsstevne iskanten 9 februar 2026</t>
         </is>
       </c>
     </row>
@@ -521,17 +521,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17:07:44</t>
+          <t>17:07:45</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Elena Sophia Sandnes-Strømmen</t>
+          <t>Aksel Eriksen</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Fana Idrettslag</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17:07:44</t>
+          <t>17:07:45</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -551,17 +551,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>17:11:28</t>
+          <t>17:11:30</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Eira Olava Bortne Ludvigsen</t>
+          <t>Frida Pasko Hansen</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Bergen Kunstløpklubb</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>17:11:28</t>
+          <t>17:11:30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -581,17 +581,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>17:15:12</t>
+          <t>17:15:15</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Sara Barbro Kyte</t>
+          <t>Angela Chen</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Bergen Kunstløpklubb</t>
+          <t>Fana Idrettslag</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17:15:12</t>
+          <t>17:15:15</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -611,17 +611,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>17:18:56</t>
+          <t>17:19:00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Mie Mariell Sævereid</t>
+          <t>Mille Isabell Steen Rein</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Bergen Kunstløpklubb</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17:18:56</t>
+          <t>17:19:00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -641,17 +641,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>17:22:40</t>
+          <t>17:22:45</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Amanda Ansnes Lima</t>
+          <t>Aylin Morseth</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Fana Idrettslag</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17:22:40</t>
+          <t>17:22:45</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -671,17 +671,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>17:26:24</t>
+          <t>17:26:30</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Emilie Morseth</t>
+          <t>Camilla Tveit</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Fana Idrettslag</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17:26:24</t>
+          <t>17:26:30</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -701,17 +701,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>17:30:08</t>
+          <t>17:30:15</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Leah Kalvik</t>
+          <t>Sara Barbro Kyte</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Bergen Kunstløpklubb</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17:30:08</t>
+          <t>17:30:15</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -731,12 +731,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>17:33:52</t>
+          <t>17:34:00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Aurelia Landschulze</t>
+          <t>Elena Sophia Sandnes-Strømmen</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -749,7 +749,7 @@
       <c r="A13" s="2" t="inlineStr"/>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>ca. 17:33:52</t>
+          <t>ca. 17:34:00</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>17:37:52</t>
+          <t>17:38:00</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>17:37:52</t>
+          <t>17:38:00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -785,12 +785,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>17:41:36</t>
+          <t>17:41:45</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Sarolt Szofia Papdi</t>
+          <t>Frida Lovisa Østerberg</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -805,7 +805,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17:41:36</t>
+          <t>17:41:45</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -815,12 +815,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>17:45:20</t>
+          <t>17:45:30</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Camilla Tveit</t>
+          <t>Amanda Ansnes Lima</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -835,7 +835,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>17:45:20</t>
+          <t>17:45:30</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -845,17 +845,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>17:49:04</t>
+          <t>17:49:15</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Hanna Wangsuk Tveita</t>
+          <t>Aurelia Landschulze</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Fana Idrettslag</t>
         </is>
       </c>
     </row>
@@ -865,7 +865,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>17:49:04</t>
+          <t>17:49:15</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -875,17 +875,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>17:52:48</t>
+          <t>17:53:00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Patricija Levickaite</t>
+          <t>Valentina Pinker-Spilde</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Bergen Kunstløpklubb</t>
+          <t>Fana Idrettslag</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>17:52:48</t>
+          <t>17:53:00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -905,12 +905,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>17:56:32</t>
+          <t>17:56:45</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Hennie Markestad</t>
+          <t>Eira Olava Bortne Ludvigsen</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17:56:32</t>
+          <t>17:56:45</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -935,12 +935,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18:00:16</t>
+          <t>18:00:30</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Yuewei Li</t>
+          <t>Sarolt Szofia Papdi</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -955,7 +955,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>18:00:16</t>
+          <t>18:00:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -965,17 +965,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>18:04:00</t>
+          <t>18:04:15</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Aylin Morseth</t>
+          <t>Mie Mariell Sævereid</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Fana Idrettslag</t>
+          <t>Bergen Kunstløpklubb</t>
         </is>
       </c>
     </row>
@@ -985,7 +985,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>18:04:00</t>
+          <t>18:04:15</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -995,17 +995,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>18:07:44</t>
+          <t>18:08:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Anne Kristoffersen</t>
+          <t>Hennie Markestad</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Bergen Kunstløpklubb</t>
         </is>
       </c>
     </row>
@@ -1013,7 +1013,7 @@
       <c r="A22" s="2" t="inlineStr"/>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>ca. 18:07:44</t>
+          <t>ca. 18:08:00</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>18:11:44</t>
+          <t>18:12:00</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>18:11:44</t>
+          <t>18:12:00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1049,17 +1049,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>18:15:28</t>
+          <t>18:15:45</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Angela Chen</t>
+          <t>Eleanora Egle</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Fana Idrettslag</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>18:15:28</t>
+          <t>18:15:45</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1079,12 +1079,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>18:19:12</t>
+          <t>18:19:30</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Frida Lovisa Østerberg</t>
+          <t>Patricija Levickaite</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>18:19:12</t>
+          <t>18:19:30</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1109,17 +1109,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>18:22:56</t>
+          <t>18:23:15</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Eleanora Egle</t>
+          <t>Yuewei Li</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Bergen Kunstløpklubb</t>
         </is>
       </c>
     </row>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>18:22:56</t>
+          <t>18:23:15</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1139,12 +1139,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>18:26:40</t>
+          <t>18:27:00</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Frida Qianlu He</t>
+          <t>Hanna Wangsuk Tveita</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>18:26:40</t>
+          <t>18:27:00</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1169,12 +1169,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>18:30:24</t>
+          <t>18:30:45</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Frida Pasko Hansen</t>
+          <t>Leah Kalvik</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>18:30:24</t>
+          <t>18:30:45</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1199,17 +1199,17 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>18:34:08</t>
+          <t>18:34:30</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Aksel Eriksen</t>
+          <t>Emilie Morseth</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Loddefjord IL</t>
+          <t>Fana Idrettslag</t>
         </is>
       </c>
     </row>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>18:34:08</t>
+          <t>18:34:30</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1229,17 +1229,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>18:37:52</t>
+          <t>18:38:15</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Valentina Pinker-Spilde</t>
+          <t>Frida Qianlu He</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Fana Idrettslag</t>
+          <t>Loddefjord IL</t>
         </is>
       </c>
     </row>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>18:37:52</t>
+          <t>18:38:15</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1259,12 +1259,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>18:41:36</t>
+          <t>18:42:00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Mille Isabell Steen Rein</t>
+          <t>Anne Kristoffersen</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1276,7 +1276,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Generert 31.01.2026 23:53</t>
+          <t>Generert 01.02.2026 08:45 • OLES_LAPTOP</t>
         </is>
       </c>
     </row>

</xml_diff>